<commit_message>
data upload and data read
</commit_message>
<xml_diff>
--- a/FinalProject/DataImporter/DataImporter.Web/wwwroot/Uploads/Users.xlsx
+++ b/FinalProject/DataImporter/DataImporter.Web/wwwroot/Uploads/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1DA612-6B5F-487B-8E08-F72DDDDB49D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E48060-A7E5-4151-9C61-393C919F3B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +65,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,7 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
@@ -107,6 +116,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -390,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -414,21 +429,124 @@
       </c>
     </row>
     <row r="2" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>1833395475</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="3" s="2" customFormat="1">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1833395475</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>